<commit_message>
🐛 Correcciones 10 de abril
</commit_message>
<xml_diff>
--- a/aplicaciones/procesador/datos/Visualización_Caracterización_20240131.xlsx
+++ b/aplicaciones/procesador/datos/Visualización_Caracterización_20240131.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CUENCO SISTEMATIZACION\SISTEMATIZACIÓN ENCUENTROS\Caracterización\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0862A9C6-42B3-42AC-B255-54F9EA2AEE80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFBA6F7-347A-4EE6-8E11-0F3C46A4B4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{57A18BAD-00D2-4856-8A10-05253F2DE6F9}"/>
   </bookViews>
@@ -1901,8 +1901,8 @@
   <dimension ref="A1:H394"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
+      <pane ySplit="1" topLeftCell="A349" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H355" sqref="H355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11086,13 +11086,13 @@
         <v>25</v>
       </c>
       <c r="F353" s="5" t="s">
-        <v>180</v>
+        <v>43</v>
       </c>
       <c r="G353" s="5" t="s">
         <v>413</v>
       </c>
       <c r="H353" s="7" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
     </row>
     <row r="354" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
@@ -11118,7 +11118,7 @@
         <v>247</v>
       </c>
       <c r="H354" s="7" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="355" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
@@ -12162,7 +12162,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H394" xr:uid="{A0DE7941-16CD-4C64-8DE2-792734A7F483}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>